<commit_message>
complete puller for exact match vendor
</commit_message>
<xml_diff>
--- a/src/assets/doc_list.xlsx
+++ b/src/assets/doc_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jason\dev\its\oi_puller\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EDAAF2-EAD4-4EE8-9564-2C96A45565C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998F606E-E8AD-4CE2-97DE-BEDC6E6749CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18570" yWindow="-6690" windowWidth="18465" windowHeight="27885" xr2:uid="{60CDEBD2-498D-49F1-83CF-F054C2CE6680}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{60CDEBD2-498D-49F1-83CF-F054C2CE6680}"/>
   </bookViews>
   <sheets>
     <sheet name="doc_list" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>invoice_num</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Test Co.</t>
+  </si>
+  <si>
+    <t>Amped Well Servicing Ltd.</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EEFD90-DD8E-4F53-B608-FBAA3FBDE296}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,6 +515,14 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>101</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -523,6 +534,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010040F83AD3462BE3458C60095CDB8EAE84" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7cfd465b8bceebafdf0dc6cec047707c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0a9c3bff-dd65-4a4d-8939-1baa60c51ca5" xmlns:ns3="0c08c633-31db-417f-b9ae-0c90af205dd5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0614d0d2e0d03692ace554c5e27ffae4" ns2:_="" ns3:_="">
     <xsd:import namespace="0a9c3bff-dd65-4a4d-8939-1baa60c51ca5"/>
@@ -751,15 +771,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -767,6 +778,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0372262-C370-459A-8607-9E498AE599EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83490346-8A60-4920-B11B-9EBF636E2DD9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -785,14 +804,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0372262-C370-459A-8607-9E498AE599EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F0369CA-839C-4CC3-8DD3-6FE6894E1C22}">
   <ds:schemaRefs>

</xml_diff>